<commit_message>
updated MCA and cleaned up source code
</commit_message>
<xml_diff>
--- a/MCA beveiligingsmethodieken.xlsx
+++ b/MCA beveiligingsmethodieken.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joasv\Documents\School\Verdieping ICT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D025CADB-341E-4AC8-8A49-749B8D4B8866}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33633E20-795E-4AFB-9921-E277752E79C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{C88D4009-2F61-4588-8BFB-5CD7A07B99EF}"/>
+    <workbookView xWindow="-5865" yWindow="-15720" windowWidth="38640" windowHeight="15840" xr2:uid="{C88D4009-2F61-4588-8BFB-5CD7A07B99EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -33,13 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="21">
-  <si>
-    <t>Confidentialty</t>
-  </si>
-  <si>
-    <t>Avalaibility</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="22">
   <si>
     <t xml:space="preserve">Reliability </t>
   </si>
@@ -53,9 +47,6 @@
     <t>Accountability</t>
   </si>
   <si>
-    <t>Intergritiy</t>
-  </si>
-  <si>
     <t xml:space="preserve">Totaal: </t>
   </si>
   <si>
@@ -68,9 +59,6 @@
     <t>Encryptie</t>
   </si>
   <si>
-    <t>Autoristatie (wachtwoorden)</t>
-  </si>
-  <si>
     <t>RFID Authenticatie</t>
   </si>
   <si>
@@ -96,6 +84,21 @@
   </si>
   <si>
     <t>Score</t>
+  </si>
+  <si>
+    <t>Confidentiality</t>
+  </si>
+  <si>
+    <t>Integrity</t>
+  </si>
+  <si>
+    <t>Availability</t>
+  </si>
+  <si>
+    <t>Autorisatie  (wachtwoorden)</t>
+  </si>
+  <si>
+    <t>Weging</t>
   </si>
 </sst>
 </file>
@@ -389,9 +392,9 @@
   <autoFilter ref="A3:F9" xr:uid="{7ED0A2CA-543F-489D-B16F-70A7EF496BF7}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{6F666E8D-B28F-48E9-AF98-8DA4E21588C0}" name="Waarde"/>
-    <tableColumn id="2" xr3:uid="{D67B58FF-50AD-4B24-9F3A-956B7E1FF8B9}" name="Confidentialty" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{88A2BCFA-A6C7-4FC8-8451-4FCB6B168058}" name="Intergritiy" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{C9430943-CB1A-4542-AA29-21C4F60DCB99}" name="Avalaibility" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{D67B58FF-50AD-4B24-9F3A-956B7E1FF8B9}" name="Confidentiality" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{88A2BCFA-A6C7-4FC8-8451-4FCB6B168058}" name="Integrity" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{C9430943-CB1A-4542-AA29-21C4F60DCB99}" name="Availability" dataDxfId="11"/>
     <tableColumn id="5" xr3:uid="{5A43D578-8707-4DE8-BF50-E91BF0A0300C}" name="Reliability " dataDxfId="10"/>
     <tableColumn id="6" xr3:uid="{F1F857FC-2B09-45A0-9DCF-3056751CC6B8}" name="Accountability " dataDxfId="9"/>
   </tableColumns>
@@ -404,9 +407,9 @@
   <autoFilter ref="A16:G22" xr:uid="{719F12B5-D8EE-4271-879B-56329F12F215}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{E9A45037-EC2C-428A-94BC-95E7F687041C}" name="Waarde"/>
-    <tableColumn id="2" xr3:uid="{0D038FD6-C082-41A0-9C26-6F1CD08F6FC1}" name="Confidentialty" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{D155D72B-097F-44DE-8496-52CB860D009F}" name="Intergritiy" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{3A2DCB25-5FC0-423A-8014-25FE4B630B96}" name="Avalaibility" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{0D038FD6-C082-41A0-9C26-6F1CD08F6FC1}" name="Confidentiality" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{D155D72B-097F-44DE-8496-52CB860D009F}" name="Integrity" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{3A2DCB25-5FC0-423A-8014-25FE4B630B96}" name="Availability" dataDxfId="6"/>
     <tableColumn id="5" xr3:uid="{6D867DED-2500-44D6-BF4F-09E26F79DC13}" name="Reliability " dataDxfId="5"/>
     <tableColumn id="6" xr3:uid="{4D4EE34F-1FE2-4B8B-9A15-F151E60FC3BC}" name="Accountability " dataDxfId="4"/>
     <tableColumn id="7" xr3:uid="{8B486D8F-0CB3-409C-ABE9-E5A98E638887}" name="rij gem."/>
@@ -420,9 +423,9 @@
   <autoFilter ref="A26:F31" xr:uid="{59EB2F1A-0C89-4CF1-A69B-A7F3A4CAECC5}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{1BAC95E4-3D29-40E4-A01D-50A9231F3FB5}" name="Waarde"/>
-    <tableColumn id="2" xr3:uid="{CC3BE9A6-FCDF-4AC4-BEFE-B268A3CC6135}" name="Confidentialty"/>
-    <tableColumn id="3" xr3:uid="{F88255F2-EC08-4334-BF72-6BBF89494CAC}" name="Intergritiy"/>
-    <tableColumn id="4" xr3:uid="{016BE4A7-F954-42BB-A23A-665360236B28}" name="Avalaibility"/>
+    <tableColumn id="2" xr3:uid="{CC3BE9A6-FCDF-4AC4-BEFE-B268A3CC6135}" name="Confidentiality"/>
+    <tableColumn id="3" xr3:uid="{F88255F2-EC08-4334-BF72-6BBF89494CAC}" name="Integrity"/>
+    <tableColumn id="4" xr3:uid="{016BE4A7-F954-42BB-A23A-665360236B28}" name="Availability"/>
     <tableColumn id="5" xr3:uid="{827D83D6-29A4-4AB0-BE24-90D1D305C67C}" name="Reliability "/>
     <tableColumn id="6" xr3:uid="{14ABB869-E6EA-4F01-BBD7-7BDFE687E15F}" name="Accountability "/>
   </tableColumns>
@@ -435,9 +438,9 @@
   <autoFilter ref="A34:F39" xr:uid="{665E044E-3B3A-4A04-81B4-CBD2D75FBECA}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{FDC9C2B9-C538-4043-BE64-11679AE4B21B}" name="Waarde"/>
-    <tableColumn id="2" xr3:uid="{018BEB8F-5287-4D29-8865-65CD52B2550B}" name="Confidentialty"/>
-    <tableColumn id="3" xr3:uid="{15AE19CA-072B-4FF3-8F72-E563F42BF0D8}" name="Intergritiy"/>
-    <tableColumn id="4" xr3:uid="{CC9E4598-0D99-478E-B17A-6FDA16B17042}" name="Avalaibility"/>
+    <tableColumn id="2" xr3:uid="{018BEB8F-5287-4D29-8865-65CD52B2550B}" name="Confidentiality"/>
+    <tableColumn id="3" xr3:uid="{15AE19CA-072B-4FF3-8F72-E563F42BF0D8}" name="Integrity"/>
+    <tableColumn id="4" xr3:uid="{CC9E4598-0D99-478E-B17A-6FDA16B17042}" name="Availability"/>
     <tableColumn id="5" xr3:uid="{202161B0-584E-408A-83C7-921078DBDDB0}" name="Reliability "/>
     <tableColumn id="6" xr3:uid="{3AB733F1-0E40-4B3B-89A8-F2DB6A56F890}" name="Accountability "/>
   </tableColumns>
@@ -450,16 +453,32 @@
   <autoFilter ref="C43:I48" xr:uid="{F98A19CA-A348-4A87-9E96-B447ECD175C4}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{3A0B56CA-4664-4FE4-938A-8EE7468EE025}" name="Waarde"/>
-    <tableColumn id="2" xr3:uid="{A1286F0A-926F-4BEF-9575-2C687F3B905E}" name="Confidentialty"/>
-    <tableColumn id="3" xr3:uid="{2D989F75-3F62-4713-9392-9303D2814118}" name="Intergritiy"/>
-    <tableColumn id="4" xr3:uid="{31D42692-4DC2-440A-9D3A-8D2B20C4A06E}" name="Avalaibility"/>
+    <tableColumn id="2" xr3:uid="{A1286F0A-926F-4BEF-9575-2C687F3B905E}" name="Confidentiality"/>
+    <tableColumn id="3" xr3:uid="{2D989F75-3F62-4713-9392-9303D2814118}" name="Integrity"/>
+    <tableColumn id="4" xr3:uid="{31D42692-4DC2-440A-9D3A-8D2B20C4A06E}" name="Availability"/>
     <tableColumn id="5" xr3:uid="{9F2B3BC8-7D84-4A5C-9693-2F900A9D4205}" name="Reliability "/>
     <tableColumn id="6" xr3:uid="{E84F3808-AC7A-48D5-9419-D4D1F7A99A3B}" name="Accountability "/>
     <tableColumn id="9" xr3:uid="{C94266CD-6E21-466F-B046-C418047EB38E}" name="Score" dataDxfId="0">
-      <calculatedColumnFormula>(Tabel356[[#This Row],[Confidentialty]]*A41)+(Tabel356[[#This Row],[Intergritiy]]*A42)+(Tabel356[[#This Row],[Avalaibility]]*A43)+(Tabel356[[#This Row],[Reliability ]]*A44)+(H44*A45)</calculatedColumnFormula>
+      <calculatedColumnFormula>(Tabel356[[#This Row],[Confidentiality]]*A41)+(Tabel356[[#This Row],[Integrity]]*A42)+(Tabel356[[#This Row],[Availability]]*A43)+(Tabel356[[#This Row],[Reliability ]]*A44)+(H44*A45)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2F1CC654-B6A4-4069-A360-6C5A7D7FF761}" name="Tabel6" displayName="Tabel6" ref="M43:S48" totalsRowShown="0">
+  <autoFilter ref="M43:S48" xr:uid="{8744E047-42C1-4FCC-9913-F3CE7EE72899}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{01657246-C8FA-4312-9D12-9931EAA4C4F8}" name="Waarde"/>
+    <tableColumn id="2" xr3:uid="{DD3EC9A4-5F61-4200-9535-4397BEB1ABB3}" name="Confidentiality"/>
+    <tableColumn id="3" xr3:uid="{7303FDE4-851F-4017-A761-2634165B8CFF}" name="Integrity"/>
+    <tableColumn id="4" xr3:uid="{1EE880AC-924B-4B00-B765-073E332A1C7E}" name="Availability"/>
+    <tableColumn id="5" xr3:uid="{652AF98E-C3D9-4D2F-9546-6581AE0A3DC6}" name="Reliability "/>
+    <tableColumn id="6" xr3:uid="{48C7D251-B5DE-449C-A0AE-8D546365B761}" name="Accountability "/>
+    <tableColumn id="7" xr3:uid="{CB1F7254-5C94-4225-9899-EE7AF92EEA65}" name="Score"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -760,17 +779,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1887DD4-2ED9-48C6-9119-371597209F26}">
-  <dimension ref="A3:I48"/>
+  <dimension ref="A3:U48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="M43" sqref="M43:S48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="13.140625" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" customWidth="1"/>
     <col min="6" max="6" width="16.28515625" customWidth="1"/>
@@ -778,31 +797,37 @@
     <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" customWidth="1"/>
+    <col min="18" max="18" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2</v>
-      </c>
       <c r="F3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -822,7 +847,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
@@ -842,7 +867,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1">
         <v>0.33300000000000002</v>
@@ -862,7 +887,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B7" s="1">
         <v>3</v>
@@ -882,7 +907,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B8" s="1">
         <v>3</v>
@@ -902,7 +927,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B9">
         <f>SUM(B4:B8)</f>
@@ -927,30 +952,30 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" t="s">
         <v>0</v>
       </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>2</v>
-      </c>
       <c r="F16" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1">
         <f>(1/9.333)</f>
@@ -978,7 +1003,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B18" s="1">
         <f>2/9.333</f>
@@ -1006,7 +1031,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B19" s="1">
         <f>0.333/9.333</f>
@@ -1034,7 +1059,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B20" s="1">
         <f>3/9.333</f>
@@ -1062,7 +1087,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B21" s="1">
         <f>3/9.333</f>
@@ -1090,7 +1115,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B22">
         <f>SUM(B17:B21)</f>
@@ -1119,127 +1144,127 @@
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="F26" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="C27" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="D27" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F27" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" t="s">
         <v>11</v>
       </c>
-      <c r="B28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" t="s">
-        <v>15</v>
-      </c>
       <c r="E28" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" t="s">
         <v>13</v>
       </c>
-      <c r="B30" t="s">
-        <v>15</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="E30" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E30" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>9</v>
-      </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="F34" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B35" s="5">
         <v>1</v>
@@ -1257,9 +1282,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B36">
         <v>0.75</v>
@@ -1277,9 +1302,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B37" s="5">
         <v>0.75</v>
@@ -1297,9 +1322,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B38">
         <v>0.25</v>
@@ -1317,38 +1342,62 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>0.17070366421689551</v>
       </c>
       <c r="C43" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D43" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G43" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="H43" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M43" t="s">
         <v>6</v>
       </c>
-      <c r="F43" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I43" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="N43" t="s">
+        <v>17</v>
+      </c>
+      <c r="O43" t="s">
+        <v>18</v>
+      </c>
+      <c r="P43" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>0</v>
+      </c>
+      <c r="R43" t="s">
+        <v>1</v>
+      </c>
+      <c r="S43" t="s">
+        <v>16</v>
+      </c>
+      <c r="U43">
+        <v>0.17070366421689601</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>0.16551735290970401</v>
       </c>
       <c r="C44" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D44" s="5">
         <v>1</v>
@@ -1366,16 +1415,40 @@
         <v>0.25</v>
       </c>
       <c r="I44">
-        <f>(Tabel356[[#This Row],[Confidentialty]]*A43)+(Tabel356[[#This Row],[Intergritiy]]*A44)+(Tabel356[[#This Row],[Avalaibility]]*A45)+(Tabel356[[#This Row],[Reliability ]]*A46)+(H44*A47)</f>
+        <f>(Tabel356[[#This Row],[Confidentiality]]*A43)+(Tabel356[[#This Row],[Integrity]]*A44)+(Tabel356[[#This Row],[Availability]]*A45)+(Tabel356[[#This Row],[Reliability ]]*A46)+(H44*A47)</f>
         <v>0.27170604361425316</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M44" t="s">
+        <v>21</v>
+      </c>
+      <c r="N44">
+        <v>0.17070366421689601</v>
+      </c>
+      <c r="O44">
+        <v>0.16551735290970401</v>
+      </c>
+      <c r="P44">
+        <v>0.26567863350790799</v>
+      </c>
+      <c r="Q44">
+        <v>0.25976946528396999</v>
+      </c>
+      <c r="R44">
+        <v>0.138330884081522</v>
+      </c>
+      <c r="S44" t="s">
+        <v>11</v>
+      </c>
+      <c r="U44">
+        <v>0.16551735290970401</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>0.26567863350790821</v>
       </c>
       <c r="C45" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D45">
         <v>0.75</v>
@@ -1393,16 +1466,40 @@
         <v>1</v>
       </c>
       <c r="I45">
-        <f>(Tabel356[[#This Row],[Confidentialty]]*A43)+(Tabel356[[#This Row],[Intergritiy]]*A44)+(Tabel356[[#This Row],[Avalaibility]]*A45)+(Tabel356[[#This Row],[Reliability ]]*A46)+(H45*A47)</f>
+        <f>(Tabel356[[#This Row],[Confidentiality]]*A43)+(Tabel356[[#This Row],[Integrity]]*A44)+(Tabel356[[#This Row],[Availability]]*A45)+(Tabel356[[#This Row],[Reliability ]]*A46)+(H45*A47)</f>
         <v>0.48047933339701554</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M45" t="s">
+        <v>7</v>
+      </c>
+      <c r="N45">
+        <v>1</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="P45">
+        <v>0.25</v>
+      </c>
+      <c r="Q45">
+        <v>0</v>
+      </c>
+      <c r="R45">
+        <v>0.25</v>
+      </c>
+      <c r="S45">
+        <v>0.27170604361425316</v>
+      </c>
+      <c r="U45">
+        <v>0.26567863350790799</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>0.25976946528396982</v>
       </c>
       <c r="C46" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D46" s="5">
         <v>0.75</v>
@@ -1420,16 +1517,40 @@
         <v>0.5</v>
       </c>
       <c r="I46">
-        <f>(Tabel356[[#This Row],[Confidentialty]]*A43)+(Tabel356[[#This Row],[Intergritiy]]*A44)+(Tabel356[[#This Row],[Avalaibility]]*A45)+(Tabel356[[#This Row],[Reliability ]]*A46)+(H46*A47)</f>
+        <f>(Tabel356[[#This Row],[Confidentiality]]*A43)+(Tabel356[[#This Row],[Integrity]]*A44)+(Tabel356[[#This Row],[Availability]]*A45)+(Tabel356[[#This Row],[Reliability ]]*A46)+(H46*A47)</f>
         <v>0.60909557443120099</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M46" t="s">
+        <v>20</v>
+      </c>
+      <c r="N46">
+        <v>0.75</v>
+      </c>
+      <c r="O46">
+        <v>0.5</v>
+      </c>
+      <c r="P46">
+        <v>0.25</v>
+      </c>
+      <c r="Q46">
+        <v>0.25</v>
+      </c>
+      <c r="R46">
+        <v>1</v>
+      </c>
+      <c r="S46">
+        <v>0.48047933339701554</v>
+      </c>
+      <c r="U46">
+        <v>0.25976946528396999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>0.13833088408152239</v>
       </c>
       <c r="C47" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D47">
         <v>0.25</v>
@@ -1447,14 +1568,59 @@
         <v>1</v>
       </c>
       <c r="I47">
-        <f>(Tabel356[[#This Row],[Confidentialty]]*A43)+(Tabel356[[#This Row],[Intergritiy]]*A44)+(Tabel356[[#This Row],[Avalaibility]]*A45)+(Tabel356[[#This Row],[Reliability ]]*A46)+(H47*A47)</f>
+        <f>(Tabel356[[#This Row],[Confidentiality]]*A43)+(Tabel356[[#This Row],[Integrity]]*A44)+(Tabel356[[#This Row],[Availability]]*A45)+(Tabel356[[#This Row],[Reliability ]]*A46)+(H47*A47)</f>
         <v>0.80555259346035124</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M47" t="s">
+        <v>8</v>
+      </c>
+      <c r="N47">
+        <v>0.75</v>
+      </c>
+      <c r="O47">
+        <v>0.5</v>
+      </c>
+      <c r="P47">
+        <v>0.75</v>
+      </c>
+      <c r="Q47">
+        <v>0.5</v>
+      </c>
+      <c r="R47">
+        <v>0.5</v>
+      </c>
+      <c r="S47">
+        <v>0.60909557443120099</v>
+      </c>
+      <c r="U47">
+        <v>0.138330884081522</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I48">
-        <f>(Tabel356[[#This Row],[Confidentialty]]*A45)+(Tabel356[[#This Row],[Intergritiy]]*A46)+(Tabel356[[#This Row],[Avalaibility]]*A47)+(Tabel356[[#This Row],[Reliability ]]*A48)+(H48*A49)</f>
+        <f>(Tabel356[[#This Row],[Confidentiality]]*A45)+(Tabel356[[#This Row],[Integrity]]*A46)+(Tabel356[[#This Row],[Availability]]*A47)+(Tabel356[[#This Row],[Reliability ]]*A48)+(H48*A49)</f>
         <v>0</v>
+      </c>
+      <c r="M48" t="s">
+        <v>9</v>
+      </c>
+      <c r="N48">
+        <v>0.25</v>
+      </c>
+      <c r="O48">
+        <v>1</v>
+      </c>
+      <c r="P48">
+        <v>0.75</v>
+      </c>
+      <c r="Q48">
+        <v>1</v>
+      </c>
+      <c r="R48">
+        <v>1</v>
+      </c>
+      <c r="S48">
+        <v>0.80555259346035124</v>
       </c>
     </row>
   </sheetData>
@@ -1462,12 +1628,13 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="5">
+  <tableParts count="6">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>